<commit_message>
updates coat of arms excel
</commit_message>
<xml_diff>
--- a/touch/data/coat-of-arms.xlsx
+++ b/touch/data/coat-of-arms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kblumenstein/Development/meeteux/meeteux-genvis/touch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{535FF027-7C59-BD4A-A339-74A52168280B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7ACD8C-60D9-7349-8270-5667F48FD036}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{199C75A8-D83E-E442-BF23-699D099CDE91}"/>
   </bookViews>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Fünf Adler Schild</t>
   </si>
@@ -77,9 +72,6 @@
     <t>Steiermark</t>
   </si>
   <si>
-    <t>Böhmische Löwenwappen</t>
-  </si>
-  <si>
     <t>Doppeladler byzant</t>
   </si>
   <si>
@@ -98,15 +90,6 @@
     <t>Thüringen</t>
   </si>
   <si>
-    <t>rot-weiß-rot/Thüringen</t>
-  </si>
-  <si>
-    <t>Mähren / rot-weiß-rot / Steiermark</t>
-  </si>
-  <si>
-    <t>rot-weiß-rot / Halicz / badisch</t>
-  </si>
-  <si>
     <t>rot-weiß-rot / Krain / Tirol / Andechs</t>
   </si>
   <si>
@@ -138,6 +121,12 @@
   </si>
   <si>
     <t>Montferrat</t>
+  </si>
+  <si>
+    <t>Number in Genealogy</t>
+  </si>
+  <si>
+    <t>id in code</t>
   </si>
 </sst>
 </file>
@@ -180,15 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -505,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DB6E45-CC71-1B44-9C1A-37BE9FB0F7E4}">
-  <dimension ref="A1:AJ41"/>
+  <dimension ref="A1:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ2" sqref="AJ2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +510,13 @@
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -568,67 +560,55 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="X1" s="1">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Y1" s="1">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="Z1" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AA1" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AB1" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AC1" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AD1" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AE1" s="1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AF1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -639,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -647,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -658,468 +638,382 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="136" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="136" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>57</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>55</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    <row r="10" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>58</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" ht="136" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>56</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" ht="136" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="11" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1">
+        <v>21</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
-        <v>57</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    </row>
+    <row r="13" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>58</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="N13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>21</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" ht="51" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>24</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
-        <v>60</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+      <c r="P16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>63</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
-        <v>24</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:31" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>61</v>
-      </c>
-      <c r="M18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>65</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1">
-        <v>62</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="S19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:31" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>64</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T23" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="U23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="V24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
+        <v>73</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>72</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1">
+        <v>46</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" ht="102" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>23</v>
-      </c>
-      <c r="B26" s="1">
+    </row>
+    <row r="30" spans="1:31" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1">
+        <v>16</v>
+      </c>
+      <c r="AC30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>66</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>67</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>21</v>
-      </c>
-      <c r="B29" s="1">
-        <v>68</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>22</v>
-      </c>
-      <c r="B30" s="1">
-        <v>69</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:31" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
+        <v>17</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1">
+        <v>48</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z33" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="119" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1">
-        <v>73</v>
-      </c>
-      <c r="AB31" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="68" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1">
-        <v>72</v>
-      </c>
-      <c r="AA32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>15</v>
-      </c>
-      <c r="AC33" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:36" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1">
-        <v>59</v>
-      </c>
-      <c r="AC34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD34" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>45</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <v>46</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:36" ht="102" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <v>16</v>
-      </c>
-      <c r="AG37" s="1" t="s">
+      <c r="AF34" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:36" ht="51" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1">
-        <v>17</v>
-      </c>
-      <c r="AH38" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1">
-        <v>48</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI39" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <v>47</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD40" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1">
-        <v>49</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ41" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds coat of arms images #5
</commit_message>
<xml_diff>
--- a/touch/data/coat-of-arms.xlsx
+++ b/touch/data/coat-of-arms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kblumenstein/Development/meeteux/meeteux-genvis/touch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7ACD8C-60D9-7349-8270-5667F48FD036}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABA5DCA-1B07-5148-A04A-7A13184B24FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{199C75A8-D83E-E442-BF23-699D099CDE91}"/>
   </bookViews>
@@ -149,12 +149,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,12 +175,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -494,20 +503,21 @@
   <dimension ref="A1:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="14.6640625" style="2" customWidth="1"/>
+    <col min="9" max="32" width="10.83203125" style="2"/>
+    <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="34" x14ac:dyDescent="0.2">
@@ -517,94 +527,94 @@
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="2">
         <v>6</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="2">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="2">
         <v>8</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="2">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="2">
         <v>10</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="2">
         <v>11</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="2">
         <v>12</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="2">
         <v>13</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="2">
         <v>14</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="2">
         <v>16</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="2">
         <v>17</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1" s="2">
         <v>18</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1" s="2">
         <v>19</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1" s="2">
         <v>20</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V1" s="2">
         <v>21</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W1" s="2">
         <v>25</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X1" s="2">
         <v>26</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y1" s="2">
         <v>27</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z1" s="2">
         <v>28</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA1" s="2">
         <v>29</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB1" s="2">
         <v>30</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC1" s="2">
         <v>31</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD1" s="2">
         <v>32</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE1" s="2">
         <v>33</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF1" s="2">
         <v>34</v>
       </c>
     </row>
@@ -615,7 +625,7 @@
       <c r="B2" s="1">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -634,7 +644,7 @@
       <c r="B4" s="1">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -645,27 +655,27 @@
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>19</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -676,7 +686,7 @@
       <c r="B7" s="1">
         <v>56</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -687,7 +697,7 @@
       <c r="B8" s="1">
         <v>57</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -706,32 +716,32 @@
       <c r="B10" s="1">
         <v>58</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>20</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>29</v>
       </c>
       <c r="B12" s="1">
         <v>21</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -742,174 +752,174 @@
       <c r="B13" s="1">
         <v>60</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>23</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>24</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>61</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>63</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="P17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>64</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>65</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="S19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>25</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>26</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>27</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="T22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>66</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="U23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>67</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="V24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>73</v>
       </c>
-      <c r="X25" s="1" t="s">
+      <c r="X25" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>72</v>
       </c>
-      <c r="W26" s="1" t="s">
+      <c r="W26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -920,7 +930,7 @@
       <c r="B27" s="1">
         <v>15</v>
       </c>
-      <c r="Y27" s="1" t="s">
+      <c r="Y27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -931,10 +941,10 @@
       <c r="B28" s="1">
         <v>45</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AA28" s="1" t="s">
+      <c r="AA28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -945,21 +955,21 @@
       <c r="B29" s="1">
         <v>46</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AB29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="102" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" ht="119" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>36</v>
       </c>
       <c r="B30" s="1">
         <v>16</v>
       </c>
-      <c r="AC30" s="1" t="s">
+      <c r="AC30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -970,7 +980,7 @@
       <c r="B31" s="1">
         <v>17</v>
       </c>
-      <c r="AD31" s="1" t="s">
+      <c r="AD31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -981,38 +991,38 @@
       <c r="B32" s="1">
         <v>48</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE32" s="1" t="s">
+      <c r="AE32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>39</v>
       </c>
       <c r="B33" s="1">
         <v>47</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z33" s="1" t="s">
+      <c r="Z33" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>40</v>
       </c>
       <c r="B34" s="1">
         <v>49</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF34" s="1" t="s">
+      <c r="AF34" s="2" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>